<commit_message>
various updates including added comments to Build.ps1
</commit_message>
<xml_diff>
--- a/My Stuff/My Tasks.xlsx
+++ b/My Stuff/My Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\MarTech\My Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4488FE-E801-4A82-868C-5E9E9030E86C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2146946-6B0B-486E-9D17-C7F9F71BC718}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="3885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>Task</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Undersand sAFE project methodology</t>
   </si>
   <si>
@@ -169,6 +166,12 @@
   </si>
   <si>
     <t>Create DBA user on GitHub.</t>
+  </si>
+  <si>
+    <t>Go throught the errors identified in GitBehaviour document and try to recreate</t>
+  </si>
+  <si>
+    <t>Understand what a Pull Request in GitHub does when it merges and when it resolves conflicts. Can all merge requests be done locally?</t>
   </si>
 </sst>
 </file>
@@ -520,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +538,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -546,235 +549,237 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -782,102 +787,120 @@
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>14</v>
+      <c r="B26" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>